<commit_message>
Added Profit column to spreadsheet
</commit_message>
<xml_diff>
--- a/PathItemData.xlsx
+++ b/PathItemData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Name of Item</t>
   </si>
@@ -25,13 +25,64 @@
     <t>Average Price in Chaos</t>
   </si>
   <si>
-    <t>Lycosidae Rawhide Tower Shield</t>
-  </si>
-  <si>
-    <t>30 chaos</t>
-  </si>
-  <si>
-    <t>18680.0307692</t>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>Starkonja's Head Silken Hood</t>
+  </si>
+  <si>
+    <t>2100.0 chaos</t>
+  </si>
+  <si>
+    <t>3136.875</t>
+  </si>
+  <si>
+    <t>1036.875</t>
+  </si>
+  <si>
+    <t>Atziri's Step Slink Boots</t>
+  </si>
+  <si>
+    <t>50 chaos</t>
+  </si>
+  <si>
+    <t>755.35</t>
+  </si>
+  <si>
+    <t>705.35</t>
+  </si>
+  <si>
+    <t>Devoto's Devotion Nightmare bascinet</t>
+  </si>
+  <si>
+    <t>420.0 chaos</t>
+  </si>
+  <si>
+    <t>4606.875</t>
+  </si>
+  <si>
+    <t>4186.875</t>
+  </si>
+  <si>
+    <t>Goldrim Leather Cap</t>
+  </si>
+  <si>
+    <t>80 chaos</t>
+  </si>
+  <si>
+    <t>145.0</t>
+  </si>
+  <si>
+    <t>65.0</t>
+  </si>
+  <si>
+    <t>Greed's Embrace Golden Plate</t>
+  </si>
+  <si>
+    <t>2765.0</t>
+  </si>
+  <si>
+    <t>665.0</t>
   </si>
 </sst>
 </file>
@@ -363,13 +414,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,16 +430,78 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>